<commit_message>
Added JTAG connector to MCU board
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Razni_projekti\VCO\VCO\ADF5355_VCO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Razni_projekti\VCO\VCO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9235E3F-9E7E-43BE-829D-FB52B7422651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B197D51D-0C34-484F-A3C2-38678BDC9306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73344E90-B40F-4A36-8DF7-D19A4216866D}"/>
+    <workbookView xWindow="6795" yWindow="1440" windowWidth="21600" windowHeight="11385" xr2:uid="{73344E90-B40F-4A36-8DF7-D19A4216866D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="111">
   <si>
     <t>Component</t>
   </si>
@@ -351,6 +351,24 @@
   </si>
   <si>
     <t>594-MCT06030C8259FP5</t>
+  </si>
+  <si>
+    <t>ARM-JTAG-20-10</t>
+  </si>
+  <si>
+    <t>Jtag adapter</t>
+  </si>
+  <si>
+    <t>Jtag 20 pin to 10 pin adapter</t>
+  </si>
+  <si>
+    <t>Jtag connector</t>
+  </si>
+  <si>
+    <t>200-SHF1101LDSMLCKTR</t>
+  </si>
+  <si>
+    <t>20 pin connector</t>
   </si>
 </sst>
 </file>
@@ -727,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD04BF4-1589-4F96-BCC7-D8F3769943E7}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,7 +817,7 @@
         <v>40</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F51" si="0">D3*E3</f>
+        <f t="shared" ref="F3:F53" si="0">D3*E3</f>
         <v>3.76</v>
       </c>
     </row>
@@ -1537,78 +1555,93 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>106</v>
+      </c>
+      <c r="B45" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" t="s">
+        <v>105</v>
+      </c>
+      <c r="D45" s="1">
+        <v>5</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
       <c r="F45" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>108</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
+        <v>110</v>
       </c>
       <c r="C46" t="s">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="D46" s="1">
-        <v>80.069999999999993</v>
+        <v>5.47</v>
       </c>
       <c r="E46">
         <v>2</v>
       </c>
       <c r="F46" s="1">
         <f t="shared" si="0"/>
+        <v>10.94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F47" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" t="s">
+        <v>44</v>
+      </c>
+      <c r="D48" s="1">
+        <v>80.069999999999993</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="0"/>
         <v>160.13999999999999</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" t="s">
-        <v>49</v>
-      </c>
-      <c r="C47" t="s">
-        <v>47</v>
-      </c>
-      <c r="D47" s="1">
-        <v>6.27</v>
-      </c>
-      <c r="E47">
-        <v>3</v>
-      </c>
-      <c r="F47" s="1">
-        <f t="shared" si="0"/>
-        <v>18.809999999999999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F48" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C49" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D49" s="1">
-        <v>16.2</v>
+        <v>6.27</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F49" s="1">
         <f t="shared" si="0"/>
-        <v>16.2</v>
+        <v>18.809999999999999</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1618,27 +1651,54 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" t="s">
+        <v>50</v>
+      </c>
+      <c r="D51" s="1">
+        <v>16.2</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
       <c r="F51" s="1">
         <f t="shared" si="0"/>
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F52" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E54" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F53" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
         <v>39</v>
       </c>
-      <c r="F54" s="1">
-        <f>SUM(F2:F51)</f>
-        <v>347.69999999999993</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E55" t="s">
+      <c r="F56" s="1">
+        <f>SUM(F2:F53)</f>
+        <v>368.64</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
         <v>40</v>
       </c>
-      <c r="F55">
-        <f>F54*7.5345</f>
-        <v>2619.7456499999998</v>
+      <c r="F57">
+        <f>F56*7.5345</f>
+        <v>2777.5180799999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a header for the VCO controls
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Razni_projekti\VCO\VCO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B197D51D-0C34-484F-A3C2-38678BDC9306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71270B79-E3CD-4242-8E7E-34F4AB3401ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6795" yWindow="1440" windowWidth="21600" windowHeight="11385" xr2:uid="{73344E90-B40F-4A36-8DF7-D19A4216866D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="114">
   <si>
     <t>Component</t>
   </si>
@@ -369,6 +369,15 @@
   </si>
   <si>
     <t>20 pin connector</t>
+  </si>
+  <si>
+    <t>855-M20-9720546</t>
+  </si>
+  <si>
+    <t>2-row 2.54mm 10 pin header</t>
+  </si>
+  <si>
+    <t>10 pin header</t>
   </si>
 </sst>
 </file>
@@ -745,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD04BF4-1589-4F96-BCC7-D8F3769943E7}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,7 +826,7 @@
         <v>40</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F53" si="0">D3*E3</f>
+        <f t="shared" ref="F3:F54" si="0">D3*E3</f>
         <v>3.76</v>
       </c>
     </row>
@@ -1597,84 +1606,99 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>113</v>
+      </c>
+      <c r="B47" t="s">
+        <v>112</v>
+      </c>
+      <c r="C47" t="s">
+        <v>111</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="E47">
+        <v>10</v>
+      </c>
       <c r="F47" s="1">
         <f t="shared" si="0"/>
+        <v>3.59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F48" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>45</v>
-      </c>
-      <c r="B48" t="s">
-        <v>46</v>
-      </c>
-      <c r="C48" t="s">
-        <v>44</v>
-      </c>
-      <c r="D48" s="1">
-        <v>80.069999999999993</v>
-      </c>
-      <c r="E48">
-        <v>2</v>
-      </c>
-      <c r="F48" s="1">
-        <f t="shared" si="0"/>
-        <v>160.13999999999999</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49" t="s">
+        <v>44</v>
+      </c>
+      <c r="D49" s="1">
+        <v>80.069999999999993</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="0"/>
+        <v>160.13999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>48</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>49</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>47</v>
       </c>
-      <c r="D49" s="1">
+      <c r="D50" s="1">
         <v>6.27</v>
       </c>
-      <c r="E49">
+      <c r="E50">
         <v>3</v>
       </c>
-      <c r="F49" s="1">
+      <c r="F50" s="1">
         <f t="shared" si="0"/>
         <v>18.809999999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F50" s="1">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F51" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>51</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>52</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>50</v>
       </c>
-      <c r="D51" s="1">
+      <c r="D52" s="1">
         <v>16.2</v>
       </c>
-      <c r="E51">
+      <c r="E52">
         <v>1</v>
       </c>
-      <c r="F51" s="1">
+      <c r="F52" s="1">
         <f t="shared" si="0"/>
         <v>16.2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F52" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1683,22 +1707,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E56" t="s">
-        <v>39</v>
-      </c>
-      <c r="F56" s="1">
-        <f>SUM(F2:F53)</f>
-        <v>368.64</v>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F54" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E57" t="s">
+        <v>39</v>
+      </c>
+      <c r="F57" s="1">
+        <f>SUM(F2:F54)</f>
+        <v>372.22999999999996</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E58" t="s">
         <v>40</v>
       </c>
-      <c r="F57">
-        <f>F56*7.5345</f>
-        <v>2777.5180799999998</v>
+      <c r="F58">
+        <f>F57*7.5345</f>
+        <v>2804.5669349999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>